<commit_message>
added more data and some diagram
</commit_message>
<xml_diff>
--- a/RQ1_Mutation/Mutation Testing Data.xlsx
+++ b/RQ1_Mutation/Mutation Testing Data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Documents\MastersDegree\CSI5370-SoftwareVerificationAndTesting\GithubRepos\csi5370project\RQ1_Mutation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F810A7A9-8568-4A7F-BA3E-03E52345D6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9285551D-8F23-4CC7-AC69-737DC6525CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="All Data" sheetId="2" r:id="rId2"/>
-    <sheet name="MutationData" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="MutationData" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="67">
   <si>
     <t>Test Suite</t>
   </si>
@@ -234,6 +235,9 @@
   <si>
     <t>Std Deviation</t>
   </si>
+  <si>
+    <t>Column1</t>
+  </si>
 </sst>
 </file>
 
@@ -253,15 +257,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -269,11 +279,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -284,11 +303,120 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -299,6 +427,1792 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ChatGPT(Implementation Based)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>P1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>P4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>P5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>P8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>P9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>P10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>P11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>P14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>P15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>P16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>P17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>P18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>P19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>P21</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>P22</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>P23</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>P24</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>P25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>P26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>P29</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>P31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>P33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>P34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>P35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>P36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>P38</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>P39</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>P40</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>P41</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>P42</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>P43</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>P44</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>P46</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>P47</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>P49</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>P50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73.209999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54.55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.709999999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.67</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61.11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41.18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40.909999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>91.18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67.739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>52.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>75.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>57.14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>77.88</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>53.92</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61.17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57.41</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>83.33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>73.77</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>83.78</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>58.75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41.67</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36.51</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>52.31</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>39.42</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15.07</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>33.33</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>32.65</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>25.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E8B-4238-804C-744A1A48E5CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ChatGPT (Description Based)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>P1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>P4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>P5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>P8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>P9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>P10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>P11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>P14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>P15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>P16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>P17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>P18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>P19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>P21</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>P22</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>P23</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>P24</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>P25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>P26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>P29</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>P31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>P33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>P34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>P35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>P36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>P38</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>P39</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>P40</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>P41</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>P42</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>P43</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>P44</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>P46</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>P47</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>P49</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>P50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.069999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.79</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42.86</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62.22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70.73</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>98.17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>66.67</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>63.16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>95.56</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>77.08</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>92.31</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>84.62</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90.91</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>98.43</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45.57</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>52.63</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>71.430000000000007</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>78.12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>64.38</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40.32</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>90.48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>93.33</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>72.97</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>63.64</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>56.92</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30.65</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>34.29</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40.78</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>54.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E8B-4238-804C-744A1A48E5CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PYNGUIN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>P1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>P4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>P5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>P8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>P9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>P10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>P11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>P14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>P15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>P16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>P17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>P18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>P19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>P21</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>P22</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>P23</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>P24</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>P25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>P26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>P29</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>P31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>P33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>P34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>P35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>P36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>P38</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>P39</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>P40</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>P41</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>P42</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>P43</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>P44</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>P46</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>P47</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>P49</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>P50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$3:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.739999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41.67</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>84.96</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39.130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21.95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>31.82</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>73.53</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30.77</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25.37</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52.63</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>79.86</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>90.48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>88.79</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>18.64</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>51.11</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>26.47</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>68.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0E8B-4238-804C-744A1A48E5CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1595781440"/>
+        <c:axId val="1595774720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1595781440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1595774720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1595774720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1595781440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>514351</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{170FDC04-2B95-388A-006F-4E18A842E63A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3682F9FE-D86D-49C3-8B86-05CCF7C6FF87}" name="Table1" displayName="Table1" ref="A2:D42" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A2:D42" xr:uid="{3682F9FE-D86D-49C3-8B86-05CCF7C6FF87}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{994A70D1-47DA-4462-8C0A-07301FF25CCE}" name="Column1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{54182D74-86D2-4B63-94B2-54967063B455}" name="ChatGPT(Implementation Based)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2BA07971-BBA7-44D4-94FF-473841396EFE}" name="ChatGPT (Description Based)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{8E4E0608-1BE7-4526-9217-88E214F410DD}" name="PYNGUIN" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4914,19 +6828,633 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1287E043-AC71-4163-8ECD-9A58D9295CF6}">
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1">
+        <v>75</v>
+      </c>
+      <c r="D3" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>61.97</v>
+      </c>
+      <c r="C4" s="1">
+        <v>70.59</v>
+      </c>
+      <c r="D4" s="1">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>65.56</v>
+      </c>
+      <c r="C5" s="1">
+        <v>74.069999999999993</v>
+      </c>
+      <c r="D5" s="1">
+        <v>18.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1">
+        <v>83.33</v>
+      </c>
+      <c r="C6" s="1">
+        <v>95.74</v>
+      </c>
+      <c r="D6" s="1">
+        <v>89.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>94.25</v>
+      </c>
+      <c r="D7" s="1">
+        <v>17.739999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1">
+        <v>73.209999999999994</v>
+      </c>
+      <c r="C8" s="1">
+        <v>67.44</v>
+      </c>
+      <c r="D8" s="1">
+        <v>25.71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>54.55</v>
+      </c>
+      <c r="C9" s="1">
+        <v>62.79</v>
+      </c>
+      <c r="D9" s="1">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1">
+        <v>55.56</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42.86</v>
+      </c>
+      <c r="D10" s="1">
+        <v>54.55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="C11" s="1">
+        <v>62.22</v>
+      </c>
+      <c r="D11" s="1">
+        <v>12.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1">
+        <v>66.67</v>
+      </c>
+      <c r="C12" s="1">
+        <v>70.73</v>
+      </c>
+      <c r="D12" s="1">
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1">
+        <v>100</v>
+      </c>
+      <c r="C13" s="1">
+        <v>98.17</v>
+      </c>
+      <c r="D13" s="1">
+        <v>15.38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1">
+        <v>80.7</v>
+      </c>
+      <c r="C14" s="1">
+        <v>66.67</v>
+      </c>
+      <c r="D14" s="1">
+        <v>41.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1">
+        <v>61.11</v>
+      </c>
+      <c r="C15" s="1">
+        <v>63.16</v>
+      </c>
+      <c r="D15" s="1">
+        <v>84.96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41.18</v>
+      </c>
+      <c r="C16" s="1">
+        <v>95.56</v>
+      </c>
+      <c r="D16" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1">
+        <v>40.909999999999997</v>
+      </c>
+      <c r="C17" s="1">
+        <v>41.3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>39.130000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1">
+        <v>91.18</v>
+      </c>
+      <c r="C18" s="1">
+        <v>77.08</v>
+      </c>
+      <c r="D18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1">
+        <v>67.739999999999995</v>
+      </c>
+      <c r="C19" s="1">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1">
+        <v>52.17</v>
+      </c>
+      <c r="C20" s="1">
+        <v>92.31</v>
+      </c>
+      <c r="D20" s="1">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1">
+        <v>75.510000000000005</v>
+      </c>
+      <c r="C21" s="1">
+        <v>84.62</v>
+      </c>
+      <c r="D21" s="1">
+        <v>21.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1">
+        <v>57.14</v>
+      </c>
+      <c r="C22" s="1">
+        <v>90.91</v>
+      </c>
+      <c r="D22" s="1">
+        <v>31.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1">
+        <v>77.88</v>
+      </c>
+      <c r="C23" s="1">
+        <v>98.43</v>
+      </c>
+      <c r="D23" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1">
+        <v>53.92</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45.57</v>
+      </c>
+      <c r="D24" s="1">
+        <v>73.53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1">
+        <v>61.17</v>
+      </c>
+      <c r="C25" s="1">
+        <v>52.63</v>
+      </c>
+      <c r="D25" s="1">
+        <v>30.77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="1">
+        <v>57.41</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44</v>
+      </c>
+      <c r="D26" s="1">
+        <v>25.37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="1">
+        <v>83.33</v>
+      </c>
+      <c r="C27" s="1">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1">
+        <v>78</v>
+      </c>
+      <c r="C28" s="1">
+        <v>78.12</v>
+      </c>
+      <c r="D28" s="1">
+        <v>52.63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="1">
+        <v>73.77</v>
+      </c>
+      <c r="C29" s="1">
+        <v>64.38</v>
+      </c>
+      <c r="D29" s="1">
+        <v>79.86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1">
+        <v>43.4</v>
+      </c>
+      <c r="C30" s="1">
+        <v>40.32</v>
+      </c>
+      <c r="D30" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="1">
+        <v>83.78</v>
+      </c>
+      <c r="C31" s="1">
+        <v>90.48</v>
+      </c>
+      <c r="D31" s="1">
+        <v>90.48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="1">
+        <v>58.75</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="D32" s="1">
+        <v>88.79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="1">
+        <v>41.67</v>
+      </c>
+      <c r="C33" s="1">
+        <v>93.33</v>
+      </c>
+      <c r="D33" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="1">
+        <v>36.51</v>
+      </c>
+      <c r="C34" s="1">
+        <v>72.97</v>
+      </c>
+      <c r="D34" s="1">
+        <v>18.64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="1">
+        <v>52.31</v>
+      </c>
+      <c r="C35" s="1">
+        <v>63.64</v>
+      </c>
+      <c r="D35" s="1">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="1">
+        <v>39.42</v>
+      </c>
+      <c r="C36" s="1">
+        <v>56.92</v>
+      </c>
+      <c r="D36" s="1">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="1">
+        <v>15.07</v>
+      </c>
+      <c r="C37" s="1">
+        <v>30.65</v>
+      </c>
+      <c r="D37" s="1">
+        <v>26.47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="1">
+        <v>33.33</v>
+      </c>
+      <c r="C38" s="1">
+        <v>34.29</v>
+      </c>
+      <c r="D38" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="1">
+        <v>32.65</v>
+      </c>
+      <c r="C39" s="1">
+        <v>40.78</v>
+      </c>
+      <c r="D39" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="1">
+        <v>25.33</v>
+      </c>
+      <c r="C40" s="1">
+        <v>54.84</v>
+      </c>
+      <c r="D40" s="1">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="8">
+        <f>AVERAGE(B6:B43)</f>
+        <v>60.024857142857151</v>
+      </c>
+      <c r="C44" s="8">
+        <f>AVERAGE(C6:C43)</f>
+        <v>65.423142857142878</v>
+      </c>
+      <c r="D44" s="8">
+        <f>AVERAGE(D6:D43)</f>
+        <v>45.314571428571426</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="9">
+        <f>_xlfn.STDEV.P(B6:B43)</f>
+        <v>19.99808481850604</v>
+      </c>
+      <c r="C45" s="9">
+        <f>_xlfn.STDEV.P(C6:C43)</f>
+        <v>22.982093622324804</v>
+      </c>
+      <c r="D45" s="9">
+        <f>_xlfn.STDEV.P(D6:D43)</f>
+        <v>26.72487918912767</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="5" t="s">
         <v>10</v>
@@ -4944,7 +7472,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -4974,7 +7502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5006,7 +7534,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -5038,7 +7566,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -5070,7 +7598,7 @@
         <v>18.18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -5102,7 +7630,7 @@
         <v>89.39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -5134,7 +7662,7 @@
         <v>17.739999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -5166,7 +7694,7 @@
         <v>25.71</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -5198,7 +7726,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -5230,7 +7758,7 @@
         <v>54.55</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -5262,7 +7790,7 @@
         <v>12.24</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -5294,7 +7822,7 @@
         <v>69.7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -5326,7 +7854,7 @@
         <v>15.38</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -5358,7 +7886,7 @@
         <v>41.67</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -5390,7 +7918,7 @@
         <v>84.96</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -5422,7 +7950,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -5454,7 +7982,7 @@
         <v>39.130000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -5486,7 +8014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -5518,7 +8046,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -5550,7 +8078,7 @@
         <v>12.12</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -5582,7 +8110,7 @@
         <v>21.95</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -5614,7 +8142,7 @@
         <v>31.82</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -5646,7 +8174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
@@ -5678,7 +8206,7 @@
         <v>73.53</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
@@ -5710,7 +8238,7 @@
         <v>30.77</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -5742,7 +8270,7 @@
         <v>25.37</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
@@ -5774,7 +8302,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
@@ -5806,7 +8334,7 @@
         <v>52.63</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>49</v>
       </c>
@@ -5838,7 +8366,7 @@
         <v>79.86</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -5870,7 +8398,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
@@ -5902,7 +8430,7 @@
         <v>90.48</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
@@ -5934,7 +8462,7 @@
         <v>88.79</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>54</v>
       </c>
@@ -5966,7 +8494,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>55</v>
       </c>
@@ -5998,7 +8526,7 @@
         <v>18.64</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>56</v>
       </c>
@@ -6030,7 +8558,7 @@
         <v>51.11</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
@@ -6062,7 +8590,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>59</v>
       </c>
@@ -6094,7 +8622,7 @@
         <v>26.47</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>60</v>
       </c>
@@ -6126,7 +8654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>62</v>
       </c>
@@ -6158,7 +8686,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>63</v>
       </c>

</xml_diff>